<commit_message>
Adding text to recent files and old files
</commit_message>
<xml_diff>
--- a/File1.xlsx
+++ b/File1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -16,6 +16,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Adding text to excel</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -144,6 +152,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -179,6 +204,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -331,12 +373,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trying for merge conflict
</commit_message>
<xml_diff>
--- a/File1.xlsx
+++ b/File1.xlsx
@@ -19,9 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Adding text to excel</t>
+  </si>
+  <si>
+    <t>Adding Conflict to git</t>
+  </si>
+  <si>
+    <t>2nd Conflict</t>
   </si>
 </sst>
 </file>
@@ -373,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G4"/>
+  <dimension ref="G4:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,6 +392,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding conflict for master
</commit_message>
<xml_diff>
--- a/File1.xlsx
+++ b/File1.xlsx
@@ -19,9 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Adding text to excel</t>
+  </si>
+  <si>
+    <t>Adding in master</t>
   </si>
 </sst>
 </file>
@@ -373,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G4"/>
+  <dimension ref="G4:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,6 +389,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>